<commit_message>
1.  Latest spreadsheets plus generated artefacts.
</commit_message>
<xml_diff>
--- a/cmip6/models/ipsl-cm6a-lr/cmip6_ipsl_ipsl-cm6a-lr_toplevel.xlsx
+++ b/cmip6/models/ipsl-cm6a-lr/cmip6_ipsl_ipsl-cm6a-lr_toplevel.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="2. Key Properties" sheetId="3" r:id="rId3"/>
     <sheet name="3. Radiative Forcings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="471">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -91,7 +91,7 @@
     <t>STRING</t>
   </si>
   <si>
-    <t>Responsible party identifiers</t>
+    <t>Mnemonic references to responsible parties</t>
   </si>
   <si>
     <t>NOTE: Multiple entries are allowed, please insert a new row per entry.</t>
@@ -103,7 +103,7 @@
     <t>Citations</t>
   </si>
   <si>
-    <t>Citation identifiers</t>
+    <t>Mnemonic references to citations</t>
   </si>
   <si>
     <t>2.1</t>
@@ -127,9 +127,6 @@
     <t>cmip6.toplevel.key_properties.name</t>
   </si>
   <si>
-    <t>IPSL-CM5A-LR;atmosphere:LMDZ5A(95x96L39);ocean:NEMOv3.2 (OPA-LIM-PISCES,149x182L31)</t>
-  </si>
-  <si>
     <t>2.1.2 *</t>
   </si>
   <si>
@@ -160,20 +157,6 @@
     <t>NOTE: Double click to expand if text is too long for cell</t>
   </si>
   <si>
-    <t>IPSL-CM5A-LR is the low resolution version of the IPSL-CM5A Earth system model. The resolution is 1.875°x3.75° with 39 vertical level for the atmosphere (96x95L39) and about 2° (with a meridional increased resolution of 0.5° near the equator) and with 31 vertical levels for the ocean (149x182L31)._x000D_
-_x000D_
-IPSL-CM5A is one of the two configurations of the IPSL-CM5 model for CMIP5, the second one being IPSL-CM5B, with a different set of atmospheric physical parameterizations._x000D_
-_x000D_
-IPSL-CM5A is an Earth system model based on an improved version of the IPSL-CM4 coupled ocean-atmosphere GCM that was used in CMIP3. Compared with IPSL-CM4, IPSL-CM5A includes among others the following improvements:_x000D_
-(i) An increase vertical resolution of the atmosphere from 19 to 39 vertical levels, with 15 levels above 20 km_x000D_
-(ii) six different species of aerosols that can be either externally prescribed or computed on-line_x000D_
-(iii) stratospheric and tropospheric ozone can be either prescribed or computed on-line_x000D_
-(iv) improved physical parameterizations of the ocean_x000D_
-(v)  carbon cycle models for both the  ocean part and  terrestrial part and land use change can be externally imposed_x000D_
-_x000D_
-More information: http://icmc.ipsl.fr/</t>
-  </si>
-  <si>
     <t>2.2</t>
   </si>
   <si>
@@ -1366,12 +1349,93 @@
   </si>
   <si>
     <t>cmip6.toplevel.radiative_forcings.other.solar.additional_information</t>
+  </si>
+  <si>
+    <t>IPSL, climate model, earth system model, LMDz atmospheric general circulation model, NEMO oceanic general circulation model, ORCHIDEE land surface model</t>
+  </si>
+  <si>
+    <t>None.</t>
+  </si>
+  <si>
+    <t>IPSL-CM4</t>
+  </si>
+  <si>
+    <t>IPSL-CM5B-LR</t>
+  </si>
+  <si>
+    <t>IPSL-CM6A-LR includes new versions of LMDz, of NEMO and of ORCHIDEE. Improved conservation of energy and water. Resolutions were increased from 96x95x39 to 144x142x79 for atmosphere and land-surface, and from 2° to 1° for ocean. The tuning phase was longer and more thorough with IPSL-CM6A-LR than with IPSL-CM5B-LR.</t>
+  </si>
+  <si>
+    <t>http://forge.ipsl.jussieu.fr/igcmg/svn/modipsl/trunk</t>
+  </si>
+  <si>
+    <t>6.1.1 to 6.1.8 with various changes in model output</t>
+  </si>
+  <si>
+    <t>shell (ksh), XML, C++ (in XIOS), Fortran90</t>
+  </si>
+  <si>
+    <t>LMDz atmospheric general circulation model and ORCHIDEE land surface model (incl. land surface carbon and a very simplified model of land ice) are grouped into a one executable (ORCHIDEE being embedded in LMDz). NEMO (ocean, sea ice, ocean biogeochemistry) is another executable. LMDz and NEMO are coupled through OASIS-MCT. XIOS (output) is a stand alone component in charge of managing all the output, driven by a set of XML files. Each of the components includes an XIOS client, that communicates to the XIOS server which flushes the output to disk.</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>The coupled model does not completely conserve energy as a number of (very) small fluxes between the components are not fully represented in the coupled model (e.g. energy flux in run-off or precipitation). Therefore the energy balance is not quite achieved, and the model equilibrates with a net top-of-atmosphere radiative imbalance of ~0.7 W.m-2.</t>
+  </si>
+  <si>
+    <t>Fluxes of latent heat, sensible heat and radiation are conserved at the atmos-ocean interface. Nevertheless fluxes of energy associated with the temperature of hydrometeors are not conserved at the surface (hydrometeors are assumed to reach the ocean surface at the sea surface (or sea-ice) temperature).</t>
+  </si>
+  <si>
+    <t>See 2.8.2.</t>
+  </si>
+  <si>
+    <t>Perfectly conserved.</t>
+  </si>
+  <si>
+    <t>Energy fluxes associated with lateral water fluxes at the land-ocean interface are not accounted for. Liquid water from river flow and coastal runoff are assumed to reach the ocean at the local SST. Iceberg (calving) are assumed to be at -4°C, and their melting is assumed to be at 0°C.</t>
+  </si>
+  <si>
+    <t>The fresh water balance was achieved to a very good precision (0.002 Sv) by ensuring quasi-conservation within each model component and across components (atmosphere-land, atmosphere-land ice, ocean-land, ocean-atmosphere).</t>
+  </si>
+  <si>
+    <t>Quasi-conserved.</t>
+  </si>
+  <si>
+    <t>Runoff is transferred to river flow and coastal runoff and is quasi-conserved into the ocean.</t>
+  </si>
+  <si>
+    <t>Snow accumulates but also evaporates over land ice. It generates iceberg calving when snowdepth exceeds a threshold. Hence freshwater is conserved when the change in snowpack over land ice is accounted for.</t>
+  </si>
+  <si>
+    <t>GHG (CO2, CH4, N2O, CFC11, CFC12 including HCFC), aerosols (sulfate, OC, BC, nitrate), radiation and cloud interactions, landuse, Ndep, stratospheric aerosols, solar</t>
+  </si>
+  <si>
+    <t>CO2, CH4, N2O, CFC11, CFC12 including HCFC</t>
+  </si>
+  <si>
+    <t>sulfate, BC, OC, nitrate, aerosol radiative effect (SW only), aerosol cloud effect</t>
+  </si>
+  <si>
+    <t>Concentrations obtained from LMDzORINCA v6 runs with interactive dust emission parametrization. Depositions obtained from LMDzORINCA v6 runs (for biogeochemistry).</t>
+  </si>
+  <si>
+    <t>CMIP6 dataset with SW/LW tailored to LMDz6 radiation transfer wavebands.</t>
+  </si>
+  <si>
+    <t>Future: return in 10 years to average historical conditions.</t>
+  </si>
+  <si>
+    <t>Obtained through LMDzORINCA v6 runs with interactive emission parametrization.</t>
+  </si>
+  <si>
+    <t>Spectral variations of solar irradiance is accounted for over the 6 model wavebands according to CMIP6 dataset v3.2.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13">
     <font>
       <sz val="11"/>
@@ -1552,11 +1616,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1630,6 +1699,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1664,6 +1734,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1839,24 +1910,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="23.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1864,7 +1935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="23.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1872,7 +1943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="23.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1880,7 +1951,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="23.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1888,7 +1959,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="23.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1896,17 +1967,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="23.25">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="23.25">
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="23.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1914,7 +1985,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="23.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -1922,7 +1993,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="23.25">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -1940,19 +2011,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="200.7109375" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
@@ -1960,7 +2031,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="18">
       <c r="A3" s="7" t="s">
         <v>21</v>
       </c>
@@ -1968,7 +2039,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
@@ -1981,10 +2052,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="18">
       <c r="B6" s="11"/>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="18">
       <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
@@ -1992,7 +2063,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="15.75">
       <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
@@ -2005,7 +2076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="18">
       <c r="B11" s="11"/>
     </row>
   </sheetData>
@@ -2014,12 +2085,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD240"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH240"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="200.7109375" customWidth="1"/>
@@ -2061,15 +2134,15 @@
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
       <c r="B6" s="11" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -2077,26 +2150,28 @@
         <v>23</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="B11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="24" customHeight="1">
       <c r="A13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -2104,41 +2179,39 @@
         <v>23</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="178" customHeight="1">
-      <c r="B16" s="11" t="s">
-        <v>47</v>
-      </c>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B16" s="11"/>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1">
       <c r="A19" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="24" customHeight="1">
       <c r="B20" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="24" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="24" customHeight="1">
@@ -2146,39 +2219,41 @@
         <v>23</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="24" customHeight="1">
       <c r="B24" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="178" customHeight="1">
-      <c r="B25" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B25" s="11" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="28" spans="1:3" ht="24" customHeight="1">
       <c r="A28" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="24" customHeight="1">
       <c r="B29" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="24" customHeight="1">
       <c r="A31" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="24" customHeight="1">
@@ -2186,21 +2261,23 @@
         <v>23</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
-      <c r="B33" s="11"/>
+      <c r="B33" s="11">
+        <v>2018</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
       <c r="A35" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="24" customHeight="1">
@@ -2208,21 +2285,23 @@
         <v>23</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="24" customHeight="1">
-      <c r="B37" s="11"/>
+      <c r="B37" s="11" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1">
       <c r="A39" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="24" customHeight="1">
@@ -2230,21 +2309,23 @@
         <v>23</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1">
-      <c r="B41" s="11"/>
+      <c r="B41" s="11" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1">
       <c r="A43" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="24" customHeight="1">
@@ -2252,26 +2333,28 @@
         <v>23</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="24" customHeight="1">
       <c r="B45" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="178" customHeight="1">
-      <c r="B46" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B46" s="11" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1">
       <c r="A48" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="24" customHeight="1">
@@ -2279,10 +2362,10 @@
         <v>23</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="24" customHeight="1">
@@ -2290,23 +2373,23 @@
     </row>
     <row r="53" spans="1:3" ht="24" customHeight="1">
       <c r="A53" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="24" customHeight="1">
       <c r="B54" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="24" customHeight="1">
       <c r="A56" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="24" customHeight="1">
@@ -2314,21 +2397,23 @@
         <v>23</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="24" customHeight="1">
-      <c r="B58" s="11"/>
+      <c r="B58" s="11" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="60" spans="1:3" ht="24" customHeight="1">
       <c r="A60" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="24" customHeight="1">
@@ -2336,21 +2421,23 @@
         <v>23</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="24" customHeight="1">
-      <c r="B62" s="11"/>
+      <c r="B62" s="11" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="64" spans="1:3" ht="24" customHeight="1">
       <c r="A64" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:34" ht="24" customHeight="1">
@@ -2358,26 +2445,28 @@
         <v>23</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:34" ht="24" customHeight="1">
       <c r="B66" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" spans="1:34" ht="24" customHeight="1">
-      <c r="B67" s="11"/>
+      <c r="B67" s="11" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="69" spans="1:34" ht="24" customHeight="1">
       <c r="A69" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="70" spans="1:34" ht="24" customHeight="1">
@@ -2385,67 +2474,71 @@
         <v>23</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="71" spans="1:34" ht="24" customHeight="1">
-      <c r="B71" s="11"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:34" ht="77.25" customHeight="1">
+      <c r="B71" s="11" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="73" spans="1:34" ht="24" customHeight="1">
       <c r="A73" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:34" ht="24" customHeight="1">
       <c r="A74" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C74" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B74" s="9" t="s">
+    </row>
+    <row r="75" spans="1:34" ht="24" customHeight="1">
+      <c r="B75" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA75" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="AB75" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="75" spans="1:34" ht="24" customHeight="1">
-      <c r="B75" s="11"/>
-      <c r="AA75" s="5" t="s">
+      <c r="AC75" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="AB75" s="5" t="s">
+      <c r="AD75" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="AC75" s="5" t="s">
+      <c r="AE75" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="AD75" s="5" t="s">
+      <c r="AF75" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="AE75" s="5" t="s">
+      <c r="AG75" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="AF75" s="5" t="s">
+      <c r="AH75" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="AG75" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="AH75" s="5" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:34" ht="24" customHeight="1">
       <c r="A78" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:34" ht="24" customHeight="1">
@@ -2453,10 +2546,10 @@
     </row>
     <row r="81" spans="1:30" ht="24" customHeight="1">
       <c r="A81" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="82" spans="1:30" ht="24" customHeight="1">
@@ -2464,10 +2557,10 @@
         <v>23</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:30" ht="24" customHeight="1">
@@ -2475,101 +2568,107 @@
     </row>
     <row r="85" spans="1:30" ht="24" customHeight="1">
       <c r="A85" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:30" ht="24" customHeight="1">
       <c r="A86" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C86" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B86" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="87" spans="1:30" ht="24" customHeight="1">
-      <c r="B87" s="11"/>
+      <c r="B87" s="11" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="89" spans="1:30" ht="24" customHeight="1">
       <c r="A89" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" spans="1:30" ht="24" customHeight="1">
       <c r="A90" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B90" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="91" spans="1:30" ht="24" customHeight="1">
+      <c r="B91" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C90" s="9" t="s">
+      <c r="AA91" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB91" s="5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="91" spans="1:30" ht="24" customHeight="1">
-      <c r="B91" s="11"/>
-      <c r="AA91" s="5" t="s">
+      <c r="AC91" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="AB91" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC91" s="5" t="s">
-        <v>126</v>
-      </c>
       <c r="AD91" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:30" ht="24" customHeight="1">
       <c r="A93" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:30" ht="24" customHeight="1">
       <c r="A94" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="95" spans="1:30" ht="24" customHeight="1">
-      <c r="B95" s="11"/>
+      <c r="B95" s="11" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="98" spans="1:3" ht="24" customHeight="1">
       <c r="A98" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="24" customHeight="1">
       <c r="B99" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="24" customHeight="1">
       <c r="A101" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="24" customHeight="1">
@@ -2577,10 +2676,10 @@
         <v>23</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="24" customHeight="1">
@@ -2588,10 +2687,10 @@
     </row>
     <row r="105" spans="1:3" ht="24" customHeight="1">
       <c r="A105" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="24" customHeight="1">
@@ -2599,26 +2698,26 @@
         <v>23</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="24" customHeight="1">
       <c r="B107" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="177.95" customHeight="1">
       <c r="B108" s="11"/>
     </row>
     <row r="110" spans="1:3" ht="24" customHeight="1">
       <c r="A110" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="24" customHeight="1">
@@ -2626,15 +2725,15 @@
         <v>23</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="24" customHeight="1">
       <c r="B112" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="24" customHeight="1">
@@ -2642,10 +2741,10 @@
     </row>
     <row r="115" spans="1:3" ht="24" customHeight="1">
       <c r="A115" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="24" customHeight="1">
@@ -2653,15 +2752,15 @@
         <v>23</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="24" customHeight="1">
       <c r="B117" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="24" customHeight="1">
@@ -2669,10 +2768,10 @@
     </row>
     <row r="120" spans="1:3" ht="24" customHeight="1">
       <c r="A120" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="24" customHeight="1">
@@ -2680,15 +2779,15 @@
         <v>23</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="24" customHeight="1">
       <c r="B122" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="24" customHeight="1">
@@ -2696,10 +2795,10 @@
     </row>
     <row r="125" spans="1:3" ht="24" customHeight="1">
       <c r="A125" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="24" customHeight="1">
@@ -2707,10 +2806,10 @@
         <v>23</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="24" customHeight="1">
@@ -2718,10 +2817,10 @@
     </row>
     <row r="129" spans="1:3" ht="24" customHeight="1">
       <c r="A129" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="24" customHeight="1">
@@ -2729,10 +2828,10 @@
         <v>23</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="24" customHeight="1">
@@ -2740,23 +2839,23 @@
     </row>
     <row r="134" spans="1:3" ht="24" customHeight="1">
       <c r="A134" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B134" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="24" customHeight="1">
       <c r="B135" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="24" customHeight="1">
       <c r="A137" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="24" customHeight="1">
@@ -2764,10 +2863,10 @@
         <v>23</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C138" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="24" customHeight="1">
@@ -2775,23 +2874,23 @@
     </row>
     <row r="142" spans="1:3" ht="24" customHeight="1">
       <c r="A142" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="24" customHeight="1">
       <c r="B143" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="24" customHeight="1">
       <c r="A145" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="24" customHeight="1">
@@ -2799,26 +2898,28 @@
         <v>23</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="24" customHeight="1">
       <c r="B147" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="178" customHeight="1">
-      <c r="B148" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B148" s="11" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="150" spans="1:3" ht="24" customHeight="1">
       <c r="A150" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="24" customHeight="1">
@@ -2826,26 +2927,28 @@
         <v>23</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="24" customHeight="1">
       <c r="B152" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="178" customHeight="1">
-      <c r="B153" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B153" s="11" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="155" spans="1:3" ht="24" customHeight="1">
       <c r="A155" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="24" customHeight="1">
@@ -2853,26 +2956,26 @@
         <v>23</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="24" customHeight="1">
       <c r="B157" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="177.95" customHeight="1">
       <c r="B158" s="11"/>
     </row>
     <row r="160" spans="1:3" ht="24" customHeight="1">
       <c r="A160" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="24" customHeight="1">
@@ -2880,26 +2983,28 @@
         <v>23</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="24" customHeight="1">
       <c r="B162" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="178" customHeight="1">
-      <c r="B163" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B163" s="11" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="165" spans="1:3" ht="24" customHeight="1">
       <c r="A165" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="24" customHeight="1">
@@ -2907,26 +3012,28 @@
         <v>23</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="24" customHeight="1">
       <c r="B167" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="178" customHeight="1">
-      <c r="B168" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B168" s="11" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="170" spans="1:3" ht="24" customHeight="1">
       <c r="A170" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="24" customHeight="1">
@@ -2934,39 +3041,41 @@
         <v>23</v>
       </c>
       <c r="B171" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="24" customHeight="1">
       <c r="B172" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="178" customHeight="1">
-      <c r="B173" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B173" s="11" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="176" spans="1:3" ht="24" customHeight="1">
       <c r="A176" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B176" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="24" customHeight="1">
       <c r="B177" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="24" customHeight="1">
       <c r="A179" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="24" customHeight="1">
@@ -2974,26 +3083,28 @@
         <v>23</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="24" customHeight="1">
       <c r="B181" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" ht="178" customHeight="1">
-      <c r="B182" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B182" s="11" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="184" spans="1:3" ht="24" customHeight="1">
       <c r="A184" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="24" customHeight="1">
@@ -3001,26 +3112,28 @@
         <v>23</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="24" customHeight="1">
       <c r="B186" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="178" customHeight="1">
-      <c r="B187" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B187" s="11" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="189" spans="1:3" ht="24" customHeight="1">
       <c r="A189" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="24" customHeight="1">
@@ -3028,26 +3141,28 @@
         <v>23</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C190" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="24" customHeight="1">
       <c r="B191" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" ht="178" customHeight="1">
-      <c r="B192" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B192" s="11" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="194" spans="1:3" ht="24" customHeight="1">
       <c r="A194" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B194" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="24" customHeight="1">
@@ -3055,26 +3170,28 @@
         <v>23</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="24" customHeight="1">
       <c r="B196" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" ht="178" customHeight="1">
-      <c r="B197" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B197" s="11" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="199" spans="1:3" ht="24" customHeight="1">
       <c r="A199" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="24" customHeight="1">
@@ -3082,26 +3199,28 @@
         <v>23</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="24" customHeight="1">
       <c r="B201" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="178" customHeight="1">
-      <c r="B202" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B202" s="11" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="204" spans="1:3" ht="24" customHeight="1">
       <c r="A204" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="24" customHeight="1">
@@ -3109,26 +3228,28 @@
         <v>23</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="24" customHeight="1">
       <c r="B206" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" ht="178" customHeight="1">
-      <c r="B207" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B207" s="11" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="209" spans="1:3" ht="24" customHeight="1">
       <c r="A209" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B209" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="24" customHeight="1">
@@ -3136,26 +3257,28 @@
         <v>23</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C210" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="24" customHeight="1">
       <c r="B211" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" ht="178" customHeight="1">
-      <c r="B212" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B212" s="11" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="214" spans="1:3" ht="24" customHeight="1">
       <c r="A214" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B214" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="24" customHeight="1">
@@ -3163,26 +3286,26 @@
         <v>23</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="24" customHeight="1">
       <c r="B216" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" ht="177.95" customHeight="1">
       <c r="B217" s="11"/>
     </row>
     <row r="219" spans="1:3" ht="24" customHeight="1">
       <c r="A219" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B219" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="24" customHeight="1">
@@ -3190,39 +3313,39 @@
         <v>23</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="24" customHeight="1">
       <c r="B221" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" ht="177.95" customHeight="1">
       <c r="B222" s="11"/>
     </row>
     <row r="225" spans="1:3" ht="24" customHeight="1">
       <c r="A225" s="12" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B225" s="12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="24" customHeight="1">
       <c r="B226" s="13" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="24" customHeight="1">
       <c r="A228" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="24" customHeight="1">
@@ -3230,39 +3353,41 @@
         <v>23</v>
       </c>
       <c r="B229" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="24" customHeight="1">
       <c r="B230" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" ht="178" customHeight="1">
-      <c r="B231" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B231" s="11" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="234" spans="1:3" ht="24" customHeight="1">
       <c r="A234" s="12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B234" s="12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="235" spans="1:3" ht="24" customHeight="1">
       <c r="B235" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="237" spans="1:3" ht="24" customHeight="1">
       <c r="A237" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B237" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="238" spans="1:3" ht="24" customHeight="1">
@@ -3270,18 +3395,18 @@
         <v>23</v>
       </c>
       <c r="B238" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="24" customHeight="1">
       <c r="B239" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" ht="177.95" customHeight="1">
       <c r="B240" s="11"/>
     </row>
   </sheetData>
@@ -3304,12 +3429,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD323"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG323"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A310" workbookViewId="0">
+      <selection activeCell="B322" sqref="B322"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="200.7109375" customWidth="1"/>
@@ -3319,20 +3446,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>33</v>
@@ -3343,10 +3470,10 @@
         <v>23</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
@@ -3354,10 +3481,10 @@
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="24" customHeight="1">
@@ -3365,39 +3492,41 @@
         <v>23</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
       <c r="B10" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B11" s="11" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:33" ht="24" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:33" ht="24" customHeight="1">
@@ -3405,45 +3534,47 @@
         <v>23</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:33" ht="24" customHeight="1">
-      <c r="B19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="22" spans="1:33" ht="24" customHeight="1">
       <c r="A22" s="12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:33" ht="24" customHeight="1">
       <c r="B23" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:33" ht="24" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:33" ht="24" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:33" ht="24" customHeight="1">
@@ -3452,35 +3583,37 @@
       </c>
     </row>
     <row r="28" spans="1:33" ht="24" customHeight="1">
-      <c r="B28" s="11"/>
+      <c r="B28" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA28" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB28" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC28" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB28" s="5" t="s">
+      <c r="AD28" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC28" s="5" t="s">
+      <c r="AE28" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD28" s="5" t="s">
+      <c r="AF28" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE28" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF28" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG28" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:33" ht="24" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31" spans="1:33" ht="24" customHeight="1">
@@ -3488,50 +3621,50 @@
         <v>23</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:33" ht="24" customHeight="1">
       <c r="B32" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" ht="177.95" customHeight="1">
       <c r="B33" s="11"/>
     </row>
     <row r="36" spans="1:33" ht="24" customHeight="1">
       <c r="A36" s="12" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37" spans="1:33" ht="24" customHeight="1">
       <c r="B37" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="39" spans="1:33" ht="24" customHeight="1">
       <c r="A39" s="7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:33" ht="24" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="41" spans="1:33" ht="24" customHeight="1">
@@ -3540,35 +3673,37 @@
       </c>
     </row>
     <row r="42" spans="1:33" ht="24" customHeight="1">
-      <c r="B42" s="11"/>
+      <c r="B42" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA42" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB42" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC42" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB42" s="5" t="s">
+      <c r="AD42" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC42" s="5" t="s">
+      <c r="AE42" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD42" s="5" t="s">
+      <c r="AF42" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE42" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF42" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG42" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:33" ht="24" customHeight="1">
       <c r="A44" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:33" ht="24" customHeight="1">
@@ -3576,50 +3711,50 @@
         <v>23</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="46" spans="1:33" ht="24" customHeight="1">
       <c r="B46" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" ht="177.95" customHeight="1">
       <c r="B47" s="11"/>
     </row>
     <row r="50" spans="1:33" ht="24" customHeight="1">
       <c r="A50" s="12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:33" ht="24" customHeight="1">
       <c r="B51" s="13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="53" spans="1:33" ht="24" customHeight="1">
       <c r="A53" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:33" ht="24" customHeight="1">
       <c r="A54" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55" spans="1:33" ht="24" customHeight="1">
@@ -3628,35 +3763,37 @@
       </c>
     </row>
     <row r="56" spans="1:33" ht="24" customHeight="1">
-      <c r="B56" s="11"/>
+      <c r="B56" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA56" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB56" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC56" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB56" s="5" t="s">
+      <c r="AD56" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC56" s="5" t="s">
+      <c r="AE56" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD56" s="5" t="s">
+      <c r="AF56" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE56" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF56" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG56" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:33" ht="24" customHeight="1">
       <c r="A58" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="59" spans="1:33" ht="24" customHeight="1">
@@ -3664,50 +3801,50 @@
         <v>23</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="60" spans="1:33" ht="24" customHeight="1">
       <c r="B60" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:33" ht="177.95" customHeight="1">
       <c r="B61" s="11"/>
     </row>
     <row r="64" spans="1:33" ht="24" customHeight="1">
       <c r="A64" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="65" spans="1:33" ht="24" customHeight="1">
       <c r="B65" s="13" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="67" spans="1:33" ht="24" customHeight="1">
       <c r="A67" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="68" spans="1:33" ht="24" customHeight="1">
       <c r="A68" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="69" spans="1:33" ht="24" customHeight="1">
@@ -3716,35 +3853,37 @@
       </c>
     </row>
     <row r="70" spans="1:33" ht="24" customHeight="1">
-      <c r="B70" s="11"/>
+      <c r="B70" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA70" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB70" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC70" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB70" s="5" t="s">
+      <c r="AD70" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC70" s="5" t="s">
+      <c r="AE70" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD70" s="5" t="s">
+      <c r="AF70" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE70" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF70" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG70" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:33" ht="24" customHeight="1">
       <c r="A72" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="73" spans="1:33" ht="24" customHeight="1">
@@ -3752,50 +3891,50 @@
         <v>23</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="74" spans="1:33" ht="24" customHeight="1">
       <c r="B74" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="75" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:33" ht="177.95" customHeight="1">
       <c r="B75" s="11"/>
     </row>
     <row r="78" spans="1:33" ht="24" customHeight="1">
       <c r="A78" s="12" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="79" spans="1:33" ht="24" customHeight="1">
       <c r="B79" s="13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="81" spans="1:33" ht="24" customHeight="1">
       <c r="A81" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="82" spans="1:33" ht="24" customHeight="1">
       <c r="A82" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:33" ht="24" customHeight="1">
@@ -3804,35 +3943,37 @@
       </c>
     </row>
     <row r="84" spans="1:33" ht="24" customHeight="1">
-      <c r="B84" s="11"/>
+      <c r="B84" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA84" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB84" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC84" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB84" s="5" t="s">
+      <c r="AD84" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC84" s="5" t="s">
+      <c r="AE84" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD84" s="5" t="s">
+      <c r="AF84" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE84" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF84" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG84" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="86" spans="1:33" ht="24" customHeight="1">
       <c r="A86" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="87" spans="1:33" ht="24" customHeight="1">
@@ -3840,50 +3981,50 @@
         <v>23</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="88" spans="1:33" ht="24" customHeight="1">
       <c r="B88" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="89" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89" spans="1:33" ht="177.95" customHeight="1">
       <c r="B89" s="11"/>
     </row>
     <row r="92" spans="1:33" ht="24" customHeight="1">
       <c r="A92" s="12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="93" spans="1:33" ht="24" customHeight="1">
       <c r="B93" s="13" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="95" spans="1:33" ht="24" customHeight="1">
       <c r="A95" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="96" spans="1:33" ht="24" customHeight="1">
       <c r="A96" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="97" spans="1:33" ht="24" customHeight="1">
@@ -3892,72 +4033,76 @@
       </c>
     </row>
     <row r="98" spans="1:33" ht="24" customHeight="1">
-      <c r="B98" s="11"/>
+      <c r="B98" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA98" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB98" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC98" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB98" s="5" t="s">
+      <c r="AD98" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC98" s="5" t="s">
+      <c r="AE98" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD98" s="5" t="s">
+      <c r="AF98" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE98" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF98" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG98" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="100" spans="1:33" ht="24" customHeight="1">
       <c r="A100" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="101" spans="1:33" ht="24" customHeight="1">
       <c r="A101" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B101" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="102" spans="1:33" ht="24" customHeight="1">
+      <c r="B102" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="AA102" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB102" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="C101" s="9" t="s">
+      <c r="AC102" s="5" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="102" spans="1:33" ht="24" customHeight="1">
-      <c r="B102" s="11"/>
-      <c r="AA102" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="AB102" s="5" t="s">
+      <c r="AD102" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="AC102" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="AD102" s="5" t="s">
-        <v>311</v>
-      </c>
       <c r="AE102" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:33" ht="24" customHeight="1">
       <c r="A104" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="105" spans="1:33" ht="24" customHeight="1">
@@ -3965,39 +4110,39 @@
         <v>23</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="106" spans="1:33" ht="24" customHeight="1">
       <c r="B106" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="107" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="107" spans="1:33" ht="177.95" customHeight="1">
       <c r="B107" s="11"/>
     </row>
     <row r="110" spans="1:33" ht="24" customHeight="1">
       <c r="A110" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="111" spans="1:33" ht="24" customHeight="1">
       <c r="B111" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="113" spans="1:33" ht="24" customHeight="1">
       <c r="A113" s="7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="114" spans="1:33" ht="24" customHeight="1">
@@ -4005,45 +4150,47 @@
         <v>23</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="115" spans="1:33" ht="24" customHeight="1">
-      <c r="B115" s="11"/>
+      <c r="B115" s="11" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="118" spans="1:33" ht="24" customHeight="1">
       <c r="A118" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="119" spans="1:33" ht="24" customHeight="1">
       <c r="B119" s="13" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="121" spans="1:33" ht="24" customHeight="1">
       <c r="A121" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="122" spans="1:33" ht="24" customHeight="1">
       <c r="A122" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="123" spans="1:33" ht="24" customHeight="1">
@@ -4052,35 +4199,37 @@
       </c>
     </row>
     <row r="124" spans="1:33" ht="24" customHeight="1">
-      <c r="B124" s="11"/>
+      <c r="B124" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA124" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB124" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC124" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB124" s="5" t="s">
+      <c r="AD124" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC124" s="5" t="s">
+      <c r="AE124" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD124" s="5" t="s">
+      <c r="AF124" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE124" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF124" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG124" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="126" spans="1:33" ht="24" customHeight="1">
       <c r="A126" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="127" spans="1:33" ht="24" customHeight="1">
@@ -4088,50 +4237,50 @@
         <v>23</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="128" spans="1:33" ht="24" customHeight="1">
       <c r="B128" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="129" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="129" spans="1:33" ht="177.95" customHeight="1">
       <c r="B129" s="11"/>
     </row>
     <row r="132" spans="1:33" ht="24" customHeight="1">
       <c r="A132" s="12" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B132" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="133" spans="1:33" ht="24" customHeight="1">
       <c r="B133" s="13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="135" spans="1:33" ht="24" customHeight="1">
       <c r="A135" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="136" spans="1:33" ht="24" customHeight="1">
       <c r="A136" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="137" spans="1:33" ht="24" customHeight="1">
@@ -4140,35 +4289,37 @@
       </c>
     </row>
     <row r="138" spans="1:33" ht="24" customHeight="1">
-      <c r="B138" s="11"/>
+      <c r="B138" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA138" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB138" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC138" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB138" s="5" t="s">
+      <c r="AD138" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC138" s="5" t="s">
+      <c r="AE138" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD138" s="5" t="s">
+      <c r="AF138" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE138" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF138" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG138" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="140" spans="1:33" ht="24" customHeight="1">
       <c r="A140" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="141" spans="1:33" ht="24" customHeight="1">
@@ -4176,50 +4327,50 @@
         <v>23</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="142" spans="1:33" ht="24" customHeight="1">
       <c r="B142" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="143" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="143" spans="1:33" ht="177.95" customHeight="1">
       <c r="B143" s="11"/>
     </row>
     <row r="146" spans="1:33" ht="24" customHeight="1">
       <c r="A146" s="12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B146" s="12" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="147" spans="1:33" ht="24" customHeight="1">
       <c r="B147" s="13" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="149" spans="1:33" ht="24" customHeight="1">
       <c r="A149" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="150" spans="1:33" ht="24" customHeight="1">
       <c r="A150" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="151" spans="1:33" ht="24" customHeight="1">
@@ -4228,35 +4379,37 @@
       </c>
     </row>
     <row r="152" spans="1:33" ht="24" customHeight="1">
-      <c r="B152" s="11"/>
+      <c r="B152" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA152" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB152" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC152" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB152" s="5" t="s">
+      <c r="AD152" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC152" s="5" t="s">
+      <c r="AE152" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD152" s="5" t="s">
+      <c r="AF152" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE152" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF152" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG152" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="154" spans="1:33" ht="24" customHeight="1">
       <c r="A154" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="155" spans="1:33" ht="24" customHeight="1">
@@ -4264,50 +4417,50 @@
         <v>23</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="156" spans="1:33" ht="24" customHeight="1">
       <c r="B156" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="157" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="157" spans="1:33" ht="177.95" customHeight="1">
       <c r="B157" s="11"/>
     </row>
     <row r="160" spans="1:33" ht="24" customHeight="1">
       <c r="A160" s="12" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B160" s="12" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="161" spans="1:33" ht="24" customHeight="1">
       <c r="B161" s="13" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="163" spans="1:33" ht="24" customHeight="1">
       <c r="A163" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="164" spans="1:33" ht="24" customHeight="1">
       <c r="A164" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="165" spans="1:33" ht="24" customHeight="1">
@@ -4316,35 +4469,37 @@
       </c>
     </row>
     <row r="166" spans="1:33" ht="24" customHeight="1">
-      <c r="B166" s="11"/>
+      <c r="B166" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA166" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB166" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC166" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB166" s="5" t="s">
+      <c r="AD166" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC166" s="5" t="s">
+      <c r="AE166" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD166" s="5" t="s">
+      <c r="AF166" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE166" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF166" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG166" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="168" spans="1:33" ht="24" customHeight="1">
       <c r="A168" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="169" spans="1:33" ht="24" customHeight="1">
@@ -4352,50 +4507,50 @@
         <v>23</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="170" spans="1:33" ht="24" customHeight="1">
       <c r="B170" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="171" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="171" spans="1:33" ht="177.95" customHeight="1">
       <c r="B171" s="11"/>
     </row>
     <row r="174" spans="1:33" ht="24" customHeight="1">
       <c r="A174" s="12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B174" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="175" spans="1:33" ht="24" customHeight="1">
       <c r="B175" s="13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="177" spans="1:33" ht="24" customHeight="1">
       <c r="A177" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="178" spans="1:33" ht="24" customHeight="1">
       <c r="A178" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="179" spans="1:33" ht="24" customHeight="1">
@@ -4404,57 +4559,61 @@
       </c>
     </row>
     <row r="180" spans="1:33" ht="24" customHeight="1">
-      <c r="B180" s="11"/>
+      <c r="B180" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA180" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB180" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC180" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB180" s="5" t="s">
+      <c r="AD180" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC180" s="5" t="s">
+      <c r="AE180" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD180" s="5" t="s">
+      <c r="AF180" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE180" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF180" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG180" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="182" spans="1:33" ht="24" customHeight="1">
       <c r="A182" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="183" spans="1:33" ht="24" customHeight="1">
       <c r="A183" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="184" spans="1:33" ht="24" customHeight="1">
-      <c r="B184" s="11"/>
+      <c r="B184" s="11" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="186" spans="1:33" ht="24" customHeight="1">
       <c r="A186" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B186" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="187" spans="1:33" ht="24" customHeight="1">
@@ -4462,50 +4621,50 @@
         <v>23</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="188" spans="1:33" ht="24" customHeight="1">
       <c r="B188" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="189" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="189" spans="1:33" ht="177.95" customHeight="1">
       <c r="B189" s="11"/>
     </row>
     <row r="192" spans="1:33" ht="24" customHeight="1">
       <c r="A192" s="12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="193" spans="1:33" ht="24" customHeight="1">
       <c r="B193" s="13" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="195" spans="1:33" ht="24" customHeight="1">
       <c r="A195" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="196" spans="1:33" ht="24" customHeight="1">
       <c r="A196" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="197" spans="1:33" ht="24" customHeight="1">
@@ -4514,79 +4673,85 @@
       </c>
     </row>
     <row r="198" spans="1:33" ht="24" customHeight="1">
-      <c r="B198" s="11"/>
+      <c r="B198" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="AA198" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB198" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC198" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB198" s="5" t="s">
+      <c r="AD198" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC198" s="5" t="s">
+      <c r="AE198" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD198" s="5" t="s">
+      <c r="AF198" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE198" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF198" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG198" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="200" spans="1:33" ht="24" customHeight="1">
       <c r="A200" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="201" spans="1:33" ht="24" customHeight="1">
       <c r="A201" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="202" spans="1:33" ht="24" customHeight="1">
-      <c r="B202" s="11"/>
+      <c r="B202" s="11" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="204" spans="1:33" ht="24" customHeight="1">
       <c r="A204" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="205" spans="1:33" ht="24" customHeight="1">
       <c r="A205" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="206" spans="1:33" ht="24" customHeight="1">
-      <c r="B206" s="11"/>
+      <c r="B206" s="11" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="208" spans="1:33" ht="24" customHeight="1">
       <c r="A208" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B208" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="209" spans="1:33" ht="24" customHeight="1">
@@ -4594,50 +4759,50 @@
         <v>23</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C209" s="9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="210" spans="1:33" ht="24" customHeight="1">
       <c r="B210" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="211" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="211" spans="1:33" ht="177.95" customHeight="1">
       <c r="B211" s="11"/>
     </row>
     <row r="214" spans="1:33" ht="24" customHeight="1">
       <c r="A214" s="12" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B214" s="12" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="215" spans="1:33" ht="24" customHeight="1">
       <c r="B215" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="217" spans="1:33" ht="24" customHeight="1">
       <c r="A217" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B217" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="218" spans="1:33" ht="24" customHeight="1">
       <c r="A218" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B218" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="219" spans="1:33" ht="24" customHeight="1">
@@ -4646,35 +4811,37 @@
       </c>
     </row>
     <row r="220" spans="1:33" ht="24" customHeight="1">
-      <c r="B220" s="11"/>
+      <c r="B220" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA220" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB220" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC220" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB220" s="5" t="s">
+      <c r="AD220" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC220" s="5" t="s">
+      <c r="AE220" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD220" s="5" t="s">
+      <c r="AF220" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE220" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF220" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG220" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="222" spans="1:33" ht="24" customHeight="1">
       <c r="A222" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B222" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="223" spans="1:33" ht="24" customHeight="1">
@@ -4682,50 +4849,52 @@
         <v>23</v>
       </c>
       <c r="B223" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C223" s="9" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="224" spans="1:33" ht="24" customHeight="1">
       <c r="B224" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="225" spans="1:33" ht="178" customHeight="1">
-      <c r="B225" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="225" spans="1:33" ht="177.95" customHeight="1">
+      <c r="B225" s="11" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="228" spans="1:33" ht="24" customHeight="1">
       <c r="A228" s="12" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B228" s="12" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="229" spans="1:33" ht="24" customHeight="1">
       <c r="B229" s="13" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="231" spans="1:33" ht="24" customHeight="1">
       <c r="A231" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="232" spans="1:33" ht="24" customHeight="1">
       <c r="A232" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B232" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="233" spans="1:33" ht="24" customHeight="1">
@@ -4734,115 +4903,127 @@
       </c>
     </row>
     <row r="234" spans="1:33" ht="24" customHeight="1">
-      <c r="B234" s="11"/>
+      <c r="B234" s="11" t="s">
+        <v>260</v>
+      </c>
       <c r="AA234" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB234" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC234" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB234" s="5" t="s">
+      <c r="AD234" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC234" s="5" t="s">
+      <c r="AE234" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD234" s="5" t="s">
+      <c r="AF234" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE234" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF234" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG234" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="236" spans="1:33" ht="24" customHeight="1">
       <c r="A236" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B236" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="237" spans="1:33" ht="24" customHeight="1">
       <c r="A237" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B237" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="C237" s="9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="238" spans="1:33" ht="24" customHeight="1">
+      <c r="B238" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D238" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AA238" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="C237" s="9" t="s">
+      <c r="AB238" s="5" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="238" spans="1:33" ht="24" customHeight="1">
-      <c r="B238" s="11"/>
-      <c r="AA238" s="5" t="s">
+      <c r="AC238" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="AB238" s="5" t="s">
+      <c r="AD238" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="AC238" s="5" t="s">
+      <c r="AE238" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="AD238" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="AE238" s="5" t="s">
-        <v>392</v>
-      </c>
       <c r="AF238" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="240" spans="1:33" ht="24" customHeight="1">
       <c r="A240" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B240" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="241" spans="1:33" ht="24" customHeight="1">
       <c r="A241" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B241" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C241" s="9" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="242" spans="1:33" ht="24" customHeight="1">
-      <c r="B242" s="11"/>
+      <c r="B242" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D242" s="5" t="s">
+        <v>260</v>
+      </c>
       <c r="AA242" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="AB242" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="AC242" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="AB242" s="5" t="s">
+      <c r="AD242" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="AC242" s="5" t="s">
+      <c r="AE242" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="AD242" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="AE242" s="5" t="s">
-        <v>392</v>
-      </c>
       <c r="AF242" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="244" spans="1:33" ht="24" customHeight="1">
       <c r="A244" s="7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B244" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="245" spans="1:33" ht="24" customHeight="1">
@@ -4850,50 +5031,50 @@
         <v>23</v>
       </c>
       <c r="B245" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="246" spans="1:33" ht="24" customHeight="1">
       <c r="B246" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="247" spans="1:33" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="247" spans="1:33" ht="177.95" customHeight="1">
       <c r="B247" s="11"/>
     </row>
     <row r="250" spans="1:33" ht="24" customHeight="1">
       <c r="A250" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B250" s="12" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="251" spans="1:33" ht="24" customHeight="1">
       <c r="B251" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="253" spans="1:33" ht="24" customHeight="1">
       <c r="A253" s="7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B253" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="254" spans="1:33" ht="24" customHeight="1">
       <c r="A254" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B254" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="255" spans="1:33" ht="24" customHeight="1">
@@ -4902,115 +5083,124 @@
       </c>
     </row>
     <row r="256" spans="1:33" ht="24" customHeight="1">
-      <c r="B256" s="11"/>
+      <c r="B256" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA256" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB256" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC256" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB256" s="5" t="s">
+      <c r="AD256" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC256" s="5" t="s">
+      <c r="AE256" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD256" s="5" t="s">
+      <c r="AF256" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE256" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF256" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG256" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="258" spans="1:32" ht="24" customHeight="1">
       <c r="A258" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B258" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="259" spans="1:32" ht="24" customHeight="1">
       <c r="A259" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B259" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="C259" s="9" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="260" spans="1:32" ht="24" customHeight="1">
+      <c r="B260" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D260" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="AA260" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="C259" s="9" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="260" spans="1:32" ht="24" customHeight="1">
-      <c r="B260" s="11"/>
-      <c r="AA260" s="5" t="s">
+      <c r="AB260" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="AC260" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="AB260" s="5" t="s">
+      <c r="AD260" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="AC260" s="5" t="s">
+      <c r="AE260" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="AD260" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="AE260" s="5" t="s">
-        <v>392</v>
-      </c>
       <c r="AF260" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="262" spans="1:32" ht="24" customHeight="1">
       <c r="A262" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B262" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="263" spans="1:32" ht="24" customHeight="1">
       <c r="A263" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B263" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C263" s="9" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="264" spans="1:32" ht="24" customHeight="1">
-      <c r="B264" s="11"/>
+      <c r="B264" s="11" t="s">
+        <v>387</v>
+      </c>
       <c r="AA264" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="AB264" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="AC264" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="AB264" s="5" t="s">
+      <c r="AD264" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="AC264" s="5" t="s">
+      <c r="AE264" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="AD264" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="AE264" s="5" t="s">
-        <v>392</v>
-      </c>
       <c r="AF264" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="266" spans="1:32" ht="24" customHeight="1">
       <c r="A266" s="7" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B266" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="267" spans="1:32" ht="24" customHeight="1">
@@ -5018,50 +5208,52 @@
         <v>23</v>
       </c>
       <c r="B267" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C267" s="9" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="268" spans="1:32" ht="24" customHeight="1">
       <c r="B268" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="269" spans="1:32" ht="178" customHeight="1">
-      <c r="B269" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="269" spans="1:32" ht="177.95" customHeight="1">
+      <c r="B269" s="11" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="272" spans="1:32" ht="24" customHeight="1">
       <c r="A272" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B272" s="12" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="273" spans="1:33" ht="24" customHeight="1">
       <c r="B273" s="13" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="275" spans="1:33" ht="24" customHeight="1">
       <c r="A275" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B275" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="276" spans="1:33" ht="24" customHeight="1">
       <c r="A276" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B276" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C276" s="9" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="277" spans="1:33" ht="24" customHeight="1">
@@ -5070,35 +5262,37 @@
       </c>
     </row>
     <row r="278" spans="1:33" ht="24" customHeight="1">
-      <c r="B278" s="11"/>
+      <c r="B278" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA278" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB278" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC278" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB278" s="5" t="s">
+      <c r="AD278" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC278" s="5" t="s">
+      <c r="AE278" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD278" s="5" t="s">
+      <c r="AF278" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE278" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF278" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG278" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="280" spans="1:33" ht="24" customHeight="1">
       <c r="A280" s="7" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B280" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="281" spans="1:33" ht="24" customHeight="1">
@@ -5106,39 +5300,41 @@
         <v>23</v>
       </c>
       <c r="B281" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C281" s="9" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="282" spans="1:33" ht="24" customHeight="1">
       <c r="B282" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="283" spans="1:33" ht="178" customHeight="1">
-      <c r="B283" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="283" spans="1:33" ht="177.95" customHeight="1">
+      <c r="B283" s="11" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="286" spans="1:33" ht="24" customHeight="1">
       <c r="A286" s="12" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B286" s="12" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="287" spans="1:33" ht="24" customHeight="1">
       <c r="B287" s="13" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="289" spans="1:33" ht="24" customHeight="1">
       <c r="A289" s="7" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B289" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="290" spans="1:33" ht="24" customHeight="1">
@@ -5146,10 +5342,10 @@
         <v>23</v>
       </c>
       <c r="B290" s="9" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C290" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="291" spans="1:33" ht="24" customHeight="1">
@@ -5157,34 +5353,34 @@
     </row>
     <row r="294" spans="1:33" ht="24" customHeight="1">
       <c r="A294" s="12" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B294" s="12" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="295" spans="1:33" ht="24" customHeight="1">
       <c r="B295" s="13" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="297" spans="1:33" ht="24" customHeight="1">
       <c r="A297" s="7" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B297" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="298" spans="1:33" ht="24" customHeight="1">
       <c r="A298" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B298" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C298" s="9" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="299" spans="1:33" ht="24" customHeight="1">
@@ -5193,57 +5389,61 @@
       </c>
     </row>
     <row r="300" spans="1:33" ht="24" customHeight="1">
-      <c r="B300" s="11"/>
+      <c r="B300" s="11" t="s">
+        <v>262</v>
+      </c>
       <c r="AA300" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AB300" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC300" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB300" s="5" t="s">
+      <c r="AD300" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC300" s="5" t="s">
+      <c r="AE300" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD300" s="5" t="s">
+      <c r="AF300" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE300" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="AF300" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="AG300" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="302" spans="1:33" ht="24" customHeight="1">
       <c r="A302" s="7" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B302" s="7" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="303" spans="1:33" ht="24" customHeight="1">
       <c r="A303" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B303" s="9" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C303" s="9" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="304" spans="1:33" ht="24" customHeight="1">
-      <c r="B304" s="11"/>
+      <c r="B304" s="11" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="306" spans="1:32" ht="24" customHeight="1">
       <c r="A306" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B306" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="307" spans="1:32" ht="24" customHeight="1">
@@ -5251,50 +5451,50 @@
         <v>23</v>
       </c>
       <c r="B307" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C307" s="9" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="308" spans="1:32" ht="24" customHeight="1">
       <c r="B308" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="309" spans="1:32" ht="178" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="309" spans="1:32" ht="177.95" customHeight="1">
       <c r="B309" s="11"/>
     </row>
     <row r="312" spans="1:32" ht="24" customHeight="1">
       <c r="A312" s="12" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B312" s="12" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="313" spans="1:32" ht="24" customHeight="1">
       <c r="B313" s="13" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="315" spans="1:32" ht="24" customHeight="1">
       <c r="A315" s="7" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B315" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="316" spans="1:32" ht="24" customHeight="1">
       <c r="A316" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B316" s="9" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C316" s="9" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="317" spans="1:32" ht="24" customHeight="1">
@@ -5303,32 +5503,34 @@
       </c>
     </row>
     <row r="318" spans="1:32" ht="24" customHeight="1">
-      <c r="B318" s="11"/>
+      <c r="B318" s="11" t="s">
+        <v>438</v>
+      </c>
       <c r="AA318" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="AB318" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="AC318" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="AD318" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="AC318" s="5" t="s">
+      <c r="AE318" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="AD318" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="AE318" s="5" t="s">
-        <v>443</v>
-      </c>
       <c r="AF318" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="320" spans="1:32" ht="24" customHeight="1">
       <c r="A320" s="7" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B320" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="321" spans="1:3" ht="24" customHeight="1">
@@ -5336,19 +5538,21 @@
         <v>23</v>
       </c>
       <c r="B321" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C321" s="9" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="322" spans="1:3" ht="24" customHeight="1">
       <c r="B322" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="323" spans="1:3" ht="178" customHeight="1">
-      <c r="B323" s="11"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B323" s="11" t="s">
+        <v>470</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="27">

</xml_diff>

<commit_message>
Updated IPSL LND and TOP spreadsheets.
</commit_message>
<xml_diff>
--- a/cmip6/models/ipsl-cm6a-lr/cmip6_ipsl_ipsl-cm6a-lr_toplevel.xlsx
+++ b/cmip6/models/ipsl-cm6a-lr/cmip6_ipsl_ipsl-cm6a-lr_toplevel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -2099,7 +2099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2184,7 +2184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH240"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
       <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>

</xml_diff>